<commit_message>
Revert "Merge branch 'master' of https://github.com/QuintusZhan/Nan_Shan_11-7"
This reverts commit e125ffd9a6ae581d609c35d792e6418ca8c45ebc, reversing
changes made to 442bc00da5e00e59f290b606c14faf9c7547d089.
</commit_message>
<xml_diff>
--- a/工作進度.xlsx
+++ b/工作進度.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FFE154-193D-6043-B4EF-EDAEE207AD71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FA2E9B-6085-5A45-99BE-3AD342455163}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="460" windowWidth="27900" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -224,13 +224,6 @@
     <t>等因變量數據完成後，完整跑一次跑回歸並完成書面報告</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
-  <si>
-    <t>12/25(三）</t>
-  </si>
-  <si>
-    <t>1.重寫PCA程式碼（之前弄到ICA去了）
-2.錄製影片</t>
-  </si>
 </sst>
 </file>
 
@@ -240,13 +233,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -319,7 +312,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -363,7 +356,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -683,11 +676,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
@@ -819,7 +812,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="95">
+    <row r="10" spans="1:7" ht="76">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -905,17 +898,6 @@
       </c>
       <c r="F18" s="2" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="38">
-      <c r="A20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>